<commit_message>
Code generation for PDU routes done
This commit includes code generation scripts to generate data structures
for PDU routes that maps Tx PDU ID to Socket ID. This commit also
includes changes to UI related to PDU Routes.
</commit_message>
<xml_diff>
--- a/tools/exacfg/analysis/AUTOSAR_SWS_SocketAdaptor.xlsx
+++ b/tools/exacfg/analysis/AUTOSAR_SWS_SocketAdaptor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\labs\zephyr-lab\Car-OS.Zephyr\car-os\tools\exacfg\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C798F23-A281-40AF-8C1F-6CA210A01FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00349507-F205-4C8E-88C9-01A1328D5348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="104">
   <si>
     <t>SoAd</t>
   </si>
@@ -332,13 +332,16 @@
   </si>
   <si>
     <t>SoAdRoutingGroupTxTriggerable</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +493,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -863,7 +873,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -873,6 +883,7 @@
     <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1235,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,7 +1255,7 @@
     <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.88671875" customWidth="1"/>
-    <col min="4" max="4" width="32.21875" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -1606,7 +1617,9 @@
       <c r="D28" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -1617,7 +1630,7 @@
       <c r="D29" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -1634,7 +1647,7 @@
       <c r="D30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1651,7 +1664,7 @@
       <c r="D31" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F31" s="5" t="s">
@@ -1668,7 +1681,7 @@
       <c r="D32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -1685,7 +1698,7 @@
       <c r="D33" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F33" s="5" t="s">
@@ -1702,7 +1715,7 @@
       <c r="D34" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -1719,7 +1732,7 @@
       <c r="D35" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F35" s="5" t="s">
@@ -1736,7 +1749,7 @@
       <c r="D36" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F36" s="5" t="s">
@@ -1753,7 +1766,7 @@
       <c r="D37" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -1770,7 +1783,7 @@
       <c r="D38" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F38" s="5" t="s">
@@ -1787,7 +1800,7 @@
       <c r="D39" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F39" s="5" t="s">
@@ -1804,7 +1817,7 @@
       <c r="D40" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -1821,7 +1834,7 @@
       <c r="D41" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F41" s="5" t="s">
@@ -1838,7 +1851,7 @@
       <c r="D42" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F42" s="5" t="s">
@@ -1855,7 +1868,7 @@
       <c r="D43" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F43" s="5"/>
@@ -1869,7 +1882,7 @@
       <c r="E44" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="9" t="s">
         <v>50</v>
       </c>
       <c r="G44" s="5" t="s">
@@ -1886,7 +1899,7 @@
       <c r="E45" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="9" t="s">
         <v>50</v>
       </c>
       <c r="G45" s="5"/>
@@ -1900,7 +1913,7 @@
       <c r="F46" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G46" s="5" t="s">
+      <c r="G46" s="9" t="s">
         <v>73</v>
       </c>
       <c r="H46" s="5" t="s">
@@ -1917,7 +1930,7 @@
       <c r="F47" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="G47" s="9" t="s">
         <v>73</v>
       </c>
       <c r="H47" s="5" t="s">
@@ -2213,6 +2226,9 @@
       <c r="D69" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E69" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D70" t="s">
@@ -2316,6 +2332,9 @@
       <c r="D77" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E77" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D78" t="s">
@@ -2460,6 +2479,9 @@
       </c>
       <c r="D88" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="E88" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>